<commit_message>
Updated project to read Locators from Excel file rather than Properties file
</commit_message>
<xml_diff>
--- a/TestSuite/TestCases.xlsx
+++ b/TestSuite/TestCases.xlsx
@@ -1,16 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26024"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25520" windowHeight="15540" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25515" windowHeight="15540" tabRatio="500"/>
   </bookViews>
   <sheets>
-    <sheet name="Test Cases" sheetId="2" r:id="rId1"/>
-    <sheet name="Test Steps" sheetId="1" r:id="rId2"/>
+    <sheet name="Test Summary" sheetId="3" r:id="rId1"/>
+    <sheet name="Test Cases" sheetId="2" r:id="rId2"/>
+    <sheet name="Test Steps" sheetId="1" r:id="rId3"/>
+    <sheet name="Page Objects" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="140000" concurrentCalc="0"/>
+  <calcPr calcId="125725" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -20,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="57">
   <si>
     <t>TestCase ID</t>
   </si>
@@ -143,13 +145,61 @@
   </si>
   <si>
     <t>No</t>
+  </si>
+  <si>
+    <t>Project</t>
+  </si>
+  <si>
+    <t>Browser</t>
+  </si>
+  <si>
+    <t>firefox</t>
+  </si>
+  <si>
+    <t>Page name</t>
+  </si>
+  <si>
+    <t>Page Object name</t>
+  </si>
+  <si>
+    <t>By</t>
+  </si>
+  <si>
+    <t>Selector</t>
+  </si>
+  <si>
+    <t>parentObject</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>password</t>
+  </si>
+  <si>
+    <t>text</t>
+  </si>
+  <si>
+    <t>Login</t>
+  </si>
+  <si>
+    <t>Login Page</t>
+  </si>
+  <si>
+    <t>Dashboard Page</t>
+  </si>
+  <si>
+    <t>Log Out</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="5">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -185,6 +235,14 @@
       <charset val="204"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -194,7 +252,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="16">
+  <borders count="17">
     <border>
       <left/>
       <right/>
@@ -361,6 +419,21 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -401,7 +474,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -423,6 +496,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="37">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -463,7 +539,24 @@
     <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="3">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
     <dxf>
       <font>
         <b/>
@@ -504,7 +597,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:D4" totalsRowShown="0" headerRowDxfId="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:D4" totalsRowShown="0" headerRowDxfId="2">
   <autoFilter ref="A1:D4"/>
   <tableColumns count="4">
     <tableColumn id="1" name="Test Case ID"/>
@@ -517,7 +610,7 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:G19" totalsRowShown="0" headerRowDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:G19" totalsRowShown="0" headerRowDxfId="1">
   <autoFilter ref="A1:G19"/>
   <tableColumns count="7">
     <tableColumn id="1" name="TestCase ID"/>
@@ -527,6 +620,20 @@
     <tableColumn id="5" name="Action_Keyword"/>
     <tableColumn id="7" name="Test_Data"/>
     <tableColumn id="6" name="Results"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table4" displayName="Table4" ref="A1:E5" totalsRowShown="0" headerRowDxfId="0">
+  <autoFilter ref="A1:E5"/>
+  <tableColumns count="5">
+    <tableColumn id="1" name="Page name"/>
+    <tableColumn id="2" name="Page Object name"/>
+    <tableColumn id="3" name="By"/>
+    <tableColumn id="4" name="Selector"/>
+    <tableColumn id="5" name="parentObject"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -853,16 +960,54 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A2:B3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75"/>
+  <cols>
+    <col min="2" max="2" width="42" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:2">
+      <c r="A2" s="22" t="s">
+        <v>41</v>
+      </c>
+      <c r="B2" s="23"/>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="22" t="s">
+        <v>42</v>
+      </c>
+      <c r="B3" s="23" t="s">
+        <v>43</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3">
+      <formula1>"chrome,ie,firefox"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="A39" sqref="A39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="24.6640625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="24.625" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="104" customWidth="1" collapsed="1"/>
     <col min="3" max="3" width="17" customWidth="1" collapsed="1"/>
   </cols>
@@ -928,25 +1073,25 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="13.33203125" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="16.6640625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="29.83203125" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="13.375" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="16.625" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="29.875" customWidth="1" collapsed="1"/>
     <col min="4" max="4" width="23.5" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="36.6640625" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="33.83203125" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="36.625" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="33.875" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="16" thickBot="1">
+    <row r="1" spans="1:7" ht="16.5" thickBot="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1068,7 +1213,7 @@
       <c r="F6" s="8"/>
       <c r="G6" s="9"/>
     </row>
-    <row r="7" spans="1:7" ht="16" thickBot="1">
+    <row r="7" spans="1:7" ht="16.5" thickBot="1">
       <c r="A7" s="10" t="s">
         <v>4</v>
       </c>
@@ -1184,7 +1329,7 @@
       <c r="F12" s="8"/>
       <c r="G12" s="9"/>
     </row>
-    <row r="13" spans="1:7" ht="16" thickBot="1">
+    <row r="13" spans="1:7" ht="16.5" thickBot="1">
       <c r="A13" s="10" t="s">
         <v>26</v>
       </c>
@@ -1300,7 +1445,7 @@
       <c r="F18" s="3"/>
       <c r="G18" s="17"/>
     </row>
-    <row r="19" spans="1:7" ht="16" thickBot="1">
+    <row r="19" spans="1:7" ht="16.5" thickBot="1">
       <c r="A19" s="18" t="s">
         <v>38</v>
       </c>
@@ -1329,4 +1474,100 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:E5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75"/>
+  <cols>
+    <col min="1" max="1" width="20.875" customWidth="1"/>
+    <col min="2" max="2" width="22.125" customWidth="1"/>
+    <col min="4" max="4" width="44.375" customWidth="1"/>
+    <col min="5" max="5" width="18.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" s="21" t="s">
+        <v>44</v>
+      </c>
+      <c r="B1" s="21" t="s">
+        <v>45</v>
+      </c>
+      <c r="C1" s="21" t="s">
+        <v>46</v>
+      </c>
+      <c r="D1" s="21" t="s">
+        <v>47</v>
+      </c>
+      <c r="E1" s="21" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" t="s">
+        <v>49</v>
+      </c>
+      <c r="D2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="B3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" t="s">
+        <v>49</v>
+      </c>
+      <c r="D3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="B4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4" t="s">
+        <v>52</v>
+      </c>
+      <c r="D4" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" t="s">
+        <v>55</v>
+      </c>
+      <c r="B5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C5" t="s">
+        <v>52</v>
+      </c>
+      <c r="D5" t="s">
+        <v>56</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C1:C1048576 C1">
+      <formula1>"xpath, css, name, id, link text, partial link text, text"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>